<commit_message>
COS Pro 2급 정리
</commit_message>
<xml_diff>
--- a/박진형.xlsx
+++ b/박진형.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dailyStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB793FA-FE33-429A-8156-D2F153DAC217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F60D089-2B51-4567-854E-C9E2CE64E56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="일정" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="138">
   <si>
     <t>해야할 일</t>
   </si>
@@ -532,11 +532,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>이현규 생일
-5시 이유진, 최상희, 김효영</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>3시 COS Pro 1급
 신촌로113 YBM신촌CBT센터</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -583,6 +578,19 @@
   </si>
   <si>
     <t>저녁 류재열?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>손정엽 결혼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이현규 생일
+6시 공덕 이유진,최상희,김효영</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심 해운대암소갈비집</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1213,7 +1221,9 @@
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <cols>
@@ -1280,16 +1290,18 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="10"/>
+        <v>128</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="50.1" customHeight="1">
       <c r="A4" s="23"/>
@@ -1330,7 +1342,7 @@
     <row r="6" spans="1:14" ht="50.1" customHeight="1">
       <c r="A6" s="23"/>
       <c r="B6" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
@@ -1344,7 +1356,7 @@
         <v>108</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="50.1" customHeight="1">
@@ -1356,7 +1368,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="35.1" customHeight="1">
@@ -1393,7 +1405,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>110</v>
@@ -1407,9 +1419,11 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="35.1" customHeight="1">
       <c r="A11" s="23"/>
@@ -1434,14 +1448,14 @@
     <row r="12" spans="1:14" ht="50.1" customHeight="1">
       <c r="A12" s="23"/>
       <c r="B12" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H12" s="10"/>
     </row>
@@ -1614,7 +1628,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H22" s="10"/>
       <c r="M22" s="4" t="s">
@@ -1705,7 +1719,7 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>

</xml_diff>

<commit_message>
COS PRO 1급 start
</commit_message>
<xml_diff>
--- a/박진형.xlsx
+++ b/박진형.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dailyStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E8EC45-9782-467E-A3A5-35D19C64EA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C951E5C-41B9-48A2-9746-D44CF90B87B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,10 +556,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>저녁 박시원</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>10시반 에어부산 김포-&gt;김해
 장전집 한솔 - 대우</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -595,6 +591,11 @@
   </si>
   <si>
     <t>10시30분 에어부산 김포-&gt;김해</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>7시 상암동 주민센터 박시원
+온돈부리 주람?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1219,9 +1220,7 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <cols>
@@ -1298,7 +1297,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="50.1" customHeight="1">
@@ -1348,7 +1347,7 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>123</v>
@@ -1462,11 +1461,11 @@
         <v>113</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M13" s="11" t="s">
         <v>74</v>
@@ -1493,7 +1492,7 @@
         <v>82</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>50</v>
@@ -1520,7 +1519,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1541,7 +1540,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H17" s="10"/>
       <c r="M17" s="11" t="s">
@@ -1587,10 +1586,10 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>81</v>
@@ -1633,7 +1632,7 @@
     <row r="22" spans="1:13" ht="50.1" customHeight="1">
       <c r="A22" s="20"/>
       <c r="B22" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1641,7 +1640,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="50.1" customHeight="1">
@@ -2098,7 +2097,7 @@
         <v>70</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>55</v>
@@ -2514,6 +2513,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F91E044E3A9D84A8197B09587594D86" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a727839579f0816cd156df87ac1abb38">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4b137422-f48a-46a4-80bc-5707d2d59248" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c55dfd8d1a660179b90c490e9dacc3e0" ns3:_="">
     <xsd:import namespace="4b137422-f48a-46a4-80bc-5707d2d59248"/>
@@ -2645,35 +2659,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD3585F-F7A7-412D-AFE1-E638B576DB58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE719ED1-0439-4266-8F9C-8738D0151331}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b137422-f48a-46a4-80bc-5707d2d59248"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2695,9 +2684,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE719ED1-0439-4266-8F9C-8738D0151331}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD3585F-F7A7-412D-AFE1-E638B576DB58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b137422-f48a-46a4-80bc-5707d2d59248"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>